<commit_message>
caracteristicas dispositivos capa 2
</commit_message>
<xml_diff>
--- a/docs/documentacion.xlsx
+++ b/docs/documentacion.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-lx10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA45CFDB-3B46-4994-BFD6-EAA0CEE9BBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7388BE36-4926-4C5C-A1FC-7F497B9D536C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" xr2:uid="{8E901FB4-342A-4602-AC7F-3C2A011F5568}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="1" xr2:uid="{8E901FB4-342A-4602-AC7F-3C2A011F5568}"/>
   </bookViews>
   <sheets>
     <sheet name="switching" sheetId="2" r:id="rId1"/>
-    <sheet name="AND" sheetId="1" r:id="rId2"/>
+    <sheet name="cisco-model" sheetId="3" r:id="rId2"/>
+    <sheet name="AND" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>AND</t>
   </si>
@@ -247,6 +248,63 @@
   </si>
   <si>
     <t>Tramas de 9KB (Config. Particular)</t>
+  </si>
+  <si>
+    <t>Escalabilidad</t>
+  </si>
+  <si>
+    <t>Tolerancia</t>
+  </si>
+  <si>
+    <t>Disponibilidad</t>
+  </si>
+  <si>
+    <t>Costos</t>
+  </si>
+  <si>
+    <t>Comandos</t>
+  </si>
+  <si>
+    <t>DUPLEX</t>
+  </si>
+  <si>
+    <t>MDIX</t>
+  </si>
+  <si>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>SWITCHPORT</t>
+  </si>
+  <si>
+    <t>Capacidad de Expansion de la topologia</t>
+  </si>
+  <si>
+    <t>Capacidad para reponerse ante un fallo</t>
+  </si>
+  <si>
+    <t>Calidad (QoS)</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Capacidad de poder establecer comunicaciones</t>
+  </si>
+  <si>
+    <t>Capacidad para identificar los mejores trayectos</t>
+  </si>
+  <si>
+    <t>Capacidad para distribuir el ancho de banda</t>
+  </si>
+  <si>
+    <t>Capacidad para prever posibles ataques</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
   </si>
 </sst>
 </file>
@@ -395,6 +453,17 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0680452A-F053-4D2D-9AC2-69AB86F49F7F}" name="TRAMAS"/>
     <tableColumn id="2" xr3:uid="{34352FC3-047F-4605-82D6-8293EF406314}" name="DETALLE"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7734FFAF-34B0-4EEB-8BC4-045D9F5DA1D8}" name="Tabla4" displayName="Tabla4" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{7734FFAF-34B0-4EEB-8BC4-045D9F5DA1D8}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A7B7EED1-968C-4B3E-BF54-AC6597CE9C21}" name="Caracteristica"/>
+    <tableColumn id="2" xr3:uid="{30EF59A4-2FC6-48F0-90A0-B032F812243F}" name="Descripcion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197C8C8A-E7B8-4205-91FD-5B11DF54B867}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A5" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +844,9 @@
       <c r="B6" t="s">
         <v>37</v>
       </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -783,6 +855,9 @@
       <c r="B7" t="s">
         <v>44</v>
       </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -791,6 +866,9 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -799,6 +877,9 @@
       <c r="B9" t="s">
         <v>45</v>
       </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -806,6 +887,9 @@
       </c>
       <c r="B10" t="s">
         <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,6 +912,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0435-9BC1-4BDD-A6D4-892202C4F888}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057F71-B3DE-434E-82DA-2F144F83FAFB}">
   <dimension ref="A1:F8"/>
   <sheetViews>

</xml_diff>

<commit_message>
tipos de vlan y enrutamiento intervlan
</commit_message>
<xml_diff>
--- a/docs/documentacion.xlsx
+++ b/docs/documentacion.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-lx10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7388BE36-4926-4C5C-A1FC-7F497B9D536C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB0560B-660E-46E3-A3B7-C77242AA9F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="1" xr2:uid="{8E901FB4-342A-4602-AC7F-3C2A011F5568}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="3" xr2:uid="{8E901FB4-342A-4602-AC7F-3C2A011F5568}"/>
   </bookViews>
   <sheets>
-    <sheet name="switching" sheetId="2" r:id="rId1"/>
-    <sheet name="cisco-model" sheetId="3" r:id="rId2"/>
-    <sheet name="AND" sheetId="1" r:id="rId3"/>
+    <sheet name="AND" sheetId="1" r:id="rId1"/>
+    <sheet name="switching" sheetId="2" r:id="rId2"/>
+    <sheet name="cisco-model" sheetId="3" r:id="rId3"/>
+    <sheet name="VLAN" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>AND</t>
   </si>
@@ -172,18 +173,9 @@
     <t>configuracion que permite utilizar varios como uno de mayor capacidad.</t>
   </si>
   <si>
-    <t>fija</t>
-  </si>
-  <si>
     <t>CONFIG</t>
   </si>
   <si>
-    <t>expandible</t>
-  </si>
-  <si>
-    <t>apilable</t>
-  </si>
-  <si>
     <t>permiten agregar otras interfaces ademas de las predeterminadas.</t>
   </si>
   <si>
@@ -196,15 +188,6 @@
     <t>DESCRIPCION</t>
   </si>
   <si>
-    <t>Metodo de Corte (cut-through)</t>
-  </si>
-  <si>
-    <t>Libre de Fragmentos (Fragment-Free)</t>
-  </si>
-  <si>
-    <t>Reenvio (Store N Forwarding)</t>
-  </si>
-  <si>
     <t>Se reenvia la trama apenas identifica la direccion mac de destino.</t>
   </si>
   <si>
@@ -274,9 +257,6 @@
     <t>SPEED</t>
   </si>
   <si>
-    <t>SWITCHPORT</t>
-  </si>
-  <si>
     <t>Capacidad de Expansion de la topologia</t>
   </si>
   <si>
@@ -305,6 +285,84 @@
   </si>
   <si>
     <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Parametros</t>
+  </si>
+  <si>
+    <t>Fija</t>
+  </si>
+  <si>
+    <t>Expandible</t>
+  </si>
+  <si>
+    <t>Apilable</t>
+  </si>
+  <si>
+    <t>Libre de Fragmentos
+(Fragment-Free)</t>
+  </si>
+  <si>
+    <t>Metodo de Corte
+(cut-through)</t>
+  </si>
+  <si>
+    <t>Almacen y Reenvio 
+(Store N Forward)</t>
+  </si>
+  <si>
+    <t>Ancho de banda (10/100/1000/AUTO)</t>
+  </si>
+  <si>
+    <t>Deteccion de interfaz cruzada (AUTO)</t>
+  </si>
+  <si>
+    <t>envio y recepcion (HALF/FULL/AUTO)</t>
+  </si>
+  <si>
+    <t>LLDP</t>
+  </si>
+  <si>
+    <t>CDP</t>
+  </si>
+  <si>
+    <t>Descubrimiento (TRANSMIT/RECEIVE)</t>
+  </si>
+  <si>
+    <t>Descubrimiento Vecino Cisco (ENABLE)</t>
+  </si>
+  <si>
+    <t>TIPOS</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>Predeterminada</t>
+  </si>
+  <si>
+    <t>Administracion</t>
+  </si>
+  <si>
+    <t>Voz</t>
+  </si>
+  <si>
+    <t>Aquella a la que se asocia el tráfico de control por defecto</t>
+  </si>
+  <si>
+    <t>Nativa</t>
+  </si>
+  <si>
+    <t>Configurada para transportar tráfico generado por usuarios</t>
+  </si>
+  <si>
+    <t>Identificador común en los extremos de un enlace troncal</t>
+  </si>
+  <si>
+    <t>SVI que posee una dirección IP y una máscara de subred</t>
+  </si>
+  <si>
+    <t>Asegura la calidad del flujo de datos de voz</t>
   </si>
 </sst>
 </file>
@@ -374,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -398,11 +456,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -426,30 +546,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66BBE75A-1BDA-4907-8C07-62AD4D016AF1}" name="Tabla1" displayName="Tabla1" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{66BBE75A-1BDA-4907-8C07-62AD4D016AF1}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BA0041CE-357C-4781-9733-9D2AE5E19858}" name="CONFIG" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{45E59AE5-2DF9-483B-9F52-B0154FD02B73}" name="CARACTERISTICA" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{898B4CB6-EB2D-462F-9900-90A3C07E2A8F}" name="Tabla7" displayName="Tabla7" ref="A1:F5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F5" xr:uid="{898B4CB6-EB2D-462F-9900-90A3C07E2A8F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8D9A98C6-4133-45C7-9A4A-6BE41C1D238F}" name="AND" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E3907926-1000-4252-916A-F65F6C963A4C}" name="Byte 1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B59F048A-76C6-491E-9D78-38D439F3A8F9}" name="Byte 2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8918CC1F-D59C-453C-9A73-31267F526449}" name="Byte 3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5AC0AE9E-F036-4A66-BA01-F07FF59049AD}" name="Byte 4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{2A1BE96E-E03B-4800-9823-B378AD9C98CC}" name="Decimal" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66BBE75A-1BDA-4907-8C07-62AD4D016AF1}" name="Tabla1" displayName="Tabla1" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{66BBE75A-1BDA-4907-8C07-62AD4D016AF1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{BA0041CE-357C-4781-9733-9D2AE5E19858}" name="CONFIG" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{45E59AE5-2DF9-483B-9F52-B0154FD02B73}" name="CARACTERISTICA" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BD2E3CC7-E24B-4B74-88AD-06FDE4769CC8}" name="Tabla2" displayName="Tabla2" ref="D1:E4" totalsRowShown="0">
   <autoFilter ref="D1:E4" xr:uid="{BD2E3CC7-E24B-4B74-88AD-06FDE4769CC8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1ACE26CA-C054-44E2-82A7-08E2782161CB}" name="METODO" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1ACE26CA-C054-44E2-82A7-08E2782161CB}" name="METODO" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{EE849693-3EDE-43B6-B147-D833E4293943}" name="DESCRIPCION"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37CBBFA6-7E54-426D-AD28-637A948C05B0}" name="Tabla3" displayName="Tabla3" ref="A6:B11" totalsRowShown="0">
-  <autoFilter ref="A6:B11" xr:uid="{37CBBFA6-7E54-426D-AD28-637A948C05B0}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37CBBFA6-7E54-426D-AD28-637A948C05B0}" name="Tabla3" displayName="Tabla3" ref="D6:E11" totalsRowShown="0">
+  <autoFilter ref="D6:E11" xr:uid="{37CBBFA6-7E54-426D-AD28-637A948C05B0}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0680452A-F053-4D2D-9AC2-69AB86F49F7F}" name="TRAMAS"/>
     <tableColumn id="2" xr3:uid="{34352FC3-047F-4605-82D6-8293EF406314}" name="DETALLE"/>
@@ -458,12 +593,34 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{87B67B44-B6A2-46D9-9C88-0F3E37D97769}" name="Tabla5" displayName="Tabla5" ref="A6:B11" totalsRowShown="0">
+  <autoFilter ref="A6:B11" xr:uid="{87B67B44-B6A2-46D9-9C88-0F3E37D97769}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3EA9EBB3-4414-48F2-B64D-A73B874D4434}" name="Comandos"/>
+    <tableColumn id="2" xr3:uid="{16BB82D3-A1B6-4C72-A6CF-B2FEBF4DD5A8}" name="Parametros"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7734FFAF-34B0-4EEB-8BC4-045D9F5DA1D8}" name="Tabla4" displayName="Tabla4" ref="A1:B7" totalsRowShown="0">
   <autoFilter ref="A1:B7" xr:uid="{7734FFAF-34B0-4EEB-8BC4-045D9F5DA1D8}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A7B7EED1-968C-4B3E-BF54-AC6597CE9C21}" name="Caracteristica"/>
     <tableColumn id="2" xr3:uid="{30EF59A4-2FC6-48F0-90A0-B032F812243F}" name="Descripcion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{95C74535-1EC8-40BD-B23C-BB5CBB2DBD36}" name="Tabla6" displayName="Tabla6" ref="A1:B6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
+  <autoFilter ref="A1:B6" xr:uid="{95C74535-1EC8-40BD-B23C-BB5CBB2DBD36}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{22C194CD-8E79-4077-A0A1-498219B0AC44}" name="TIPOS" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{5E1B5D58-7BF0-4169-B98B-A83EC52EA46C}" name="Descripcion" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -765,236 +922,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197C8C8A-E7B8-4205-91FD-5B11DF54B867}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="2.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0435-9BC1-4BDD-A6D4-892202C4F888}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057F71-B3DE-434E-82DA-2F144F83FAFB}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,5 +1043,343 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197C8C8A-E7B8-4205-91FD-5B11DF54B867}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0435-9BC1-4BDD-A6D4-892202C4F888}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA26138-7E8A-4EEE-B2C1-31CE892488B6}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="11.42578125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>